<commit_message>
Rescaling the BFI scores to 1-10 + added more tests
</commit_message>
<xml_diff>
--- a/PeerJ-LS2022/Experiment-PeerJ-LS2022-backup.xlsx
+++ b/PeerJ-LS2022/Experiment-PeerJ-LS2022-backup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelv/Documents/legal/school/PeerJ/experimental-scripts/PeerJ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelv/Documents/legal/school/A*-Studie/PeerJ'24 - LS2022+cross/experimental-scripts/PeerJ-LS2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97A9198-1A2E-8E43-BDBE-65EABDB206C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1498287-37A7-E64E-8AA4-0295375A56F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="760" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:BP78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BI40" workbookViewId="0">
-      <selection activeCell="BM53" sqref="BM53"/>
+      <selection activeCell="BO46" sqref="BO46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>